<commit_message>
ADDED TIMER, TIME-STAMP IN DATABASE AS WELL
</commit_message>
<xml_diff>
--- a/time_sheet/timeSheet.xlsx
+++ b/time_sheet/timeSheet.xlsx
@@ -182,11 +182,11 @@
   </sheetPr>
   <dimension ref="A1:F162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A129" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E149" activeCellId="0" sqref="E149"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F144" activeCellId="0" sqref="F144"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="16.43"/>
   </cols>
@@ -3225,14 +3225,14 @@
         <v>15</v>
       </c>
       <c r="D145" s="0" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E145" s="0" t="n">
         <v>1500</v>
       </c>
       <c r="F145" s="0" t="n">
         <f aca="false">D145*E145</f>
-        <v>0</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3579,12 +3579,12 @@
       <c r="C162" s="1"/>
       <c r="D162" s="2" t="n">
         <f aca="false">SUM(D2:D161)</f>
-        <v>74.5</v>
+        <v>79.5</v>
       </c>
       <c r="E162" s="3"/>
       <c r="F162" s="0" t="n">
         <f aca="false">SUM(F2:F161)</f>
-        <v>111750</v>
+        <v>119250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>